<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@33efd0782432cc1ab567b11091fbf0c125c11d0e 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="959" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80B4F4BE-717B-4BE3-AFD3-3661C1CF11A2}"/>
+  <xr:revisionPtr revIDLastSave="960" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C9A215-DCD9-4209-8534-3CFA4DEA7823}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="33710" windowHeight="14000" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
@@ -1483,9 +1483,6 @@
     <t>Evaluating the contribution of cell-type specific alternative splicing to variation in lipid levels</t>
   </si>
   <si>
-    <t>Natural human genetic variation determines basal and inducible expression  ofnPM20D1n  an obesity-associated gene</t>
-  </si>
-  <si>
     <t>Postmenopausal osteoporotic fracture-associated COLIA1 variant impacts bone accretion in girls</t>
   </si>
   <si>
@@ -1895,6 +1892,9 @@
   </si>
   <si>
     <t>https://journals.plos.org/plosgenetics/article/file?id=10.1371/journal.pgen.0010032&amp;type=printable</t>
+  </si>
+  <si>
+    <t>Natural human genetic variation determines basal and inducible expression  of PM20D1 an obesity-associated gene</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +1965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1985,7 +1985,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4726,8 +4725,8 @@
   <dimension ref="A1:AG214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -4772,7 +4771,7 @@
         <v>187</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>190</v>
@@ -4790,28 +4789,28 @@
         <v>416</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>164</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>575</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>169</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>171</v>
@@ -4823,7 +4822,7 @@
         <v>173</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>175</v>
@@ -4847,19 +4846,19 @@
         <v>181</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>183</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>185</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AG1" s="4" t="s">
         <v>404</v>
@@ -5984,7 +5983,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>431</v>
@@ -5993,7 +5992,7 @@
         <v>2023</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>162</v>
@@ -6088,7 +6087,7 @@
         <v>162</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E14" s="3">
         <v>2023</v>
@@ -6391,16 +6390,16 @@
         <v>162</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E17" s="3">
         <v>2022</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>162</v>
@@ -6590,7 +6589,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>434</v>
@@ -6599,10 +6598,10 @@
         <v>2022</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>162</v>
@@ -6792,7 +6791,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>435</v>
@@ -6804,7 +6803,7 @@
         <v>162</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>162</v>
@@ -6896,7 +6895,7 @@
         <v>162</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E22" s="3">
         <v>2022</v>
@@ -6905,7 +6904,7 @@
         <v>162</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>162</v>
@@ -6994,7 +6993,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>436</v>
@@ -7006,7 +7005,7 @@
         <v>162</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>162</v>
@@ -7095,7 +7094,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>437</v>
@@ -7107,7 +7106,7 @@
         <v>162</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>162</v>
@@ -7297,7 +7296,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>439</v>
@@ -8007,7 +8006,7 @@
         <v>162</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E33" s="3">
         <v>2021</v>
@@ -8613,7 +8612,7 @@
         <v>162</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E39" s="3">
         <v>2021</v>
@@ -13259,7 +13258,7 @@
         <v>162</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>480</v>
+        <v>617</v>
       </c>
       <c r="E85" s="3">
         <v>2019</v>
@@ -13360,7 +13359,7 @@
         <v>162</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E86" s="3">
         <v>2019</v>
@@ -13461,7 +13460,7 @@
         <v>162</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E87" s="3">
         <v>2019</v>
@@ -13562,7 +13561,7 @@
         <v>162</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E88" s="3">
         <v>2019</v>
@@ -13764,7 +13763,7 @@
         <v>162</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E90" s="3">
         <v>2018</v>
@@ -13966,7 +13965,7 @@
         <v>162</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E92" s="3">
         <v>2018</v>
@@ -14168,7 +14167,7 @@
         <v>162</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E94" s="3">
         <v>2018</v>
@@ -14269,7 +14268,7 @@
         <v>162</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E95" s="3">
         <v>2018</v>
@@ -14370,7 +14369,7 @@
         <v>162</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E96" s="3">
         <v>2018</v>
@@ -14471,7 +14470,7 @@
         <v>162</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E97" s="3">
         <v>2018</v>
@@ -14572,7 +14571,7 @@
         <v>162</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E98" s="3">
         <v>2017</v>
@@ -14673,7 +14672,7 @@
         <v>162</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E99" s="3">
         <v>2018</v>
@@ -14976,7 +14975,7 @@
         <v>162</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E102" s="3">
         <v>2017</v>
@@ -15077,7 +15076,7 @@
         <v>162</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E103" s="3">
         <v>2017</v>
@@ -15481,7 +15480,7 @@
         <v>162</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E107" s="3">
         <v>2017</v>
@@ -15582,7 +15581,7 @@
         <v>162</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E108" s="3">
         <v>2017</v>
@@ -15683,7 +15682,7 @@
         <v>162</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E109" s="3">
         <v>2017</v>
@@ -15784,7 +15783,7 @@
         <v>162</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E110" s="3">
         <v>2017</v>
@@ -15986,7 +15985,7 @@
         <v>162</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E112" s="3">
         <v>2016</v>
@@ -16087,7 +16086,7 @@
         <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E113" s="3">
         <v>2017</v>
@@ -16188,7 +16187,7 @@
         <v>162</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E114" s="3">
         <v>2016</v>
@@ -16289,7 +16288,7 @@
         <v>162</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E115" s="3">
         <v>2016</v>
@@ -16390,7 +16389,7 @@
         <v>162</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E116" s="3">
         <v>2016</v>
@@ -16491,7 +16490,7 @@
         <v>162</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E117" s="3">
         <v>2016</v>
@@ -16895,7 +16894,7 @@
         <v>162</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E121" s="3">
         <v>2016</v>
@@ -17097,7 +17096,7 @@
         <v>162</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E123" s="3">
         <v>2016</v>
@@ -17299,7 +17298,7 @@
         <v>162</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E125" s="3">
         <v>2015</v>
@@ -17400,7 +17399,7 @@
         <v>162</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E126" s="3">
         <v>2015</v>
@@ -17501,7 +17500,7 @@
         <v>162</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E127" s="3">
         <v>2015</v>
@@ -17905,7 +17904,7 @@
         <v>162</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E131" s="3">
         <v>2014</v>
@@ -18410,7 +18409,7 @@
         <v>162</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E136" s="3">
         <v>2014</v>
@@ -18612,7 +18611,7 @@
         <v>162</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E138" s="3">
         <v>2013</v>
@@ -18915,7 +18914,7 @@
         <v>162</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E141" s="3">
         <v>2013</v>
@@ -19117,7 +19116,7 @@
         <v>162</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E143" s="3">
         <v>2012</v>
@@ -19218,7 +19217,7 @@
         <v>162</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E144" s="3">
         <v>2013</v>
@@ -19521,7 +19520,7 @@
         <v>162</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E147" s="3">
         <v>2012</v>
@@ -19925,7 +19924,7 @@
         <v>162</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E151" s="3">
         <v>2012</v>
@@ -20026,7 +20025,7 @@
         <v>162</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E152" s="3">
         <v>2012</v>
@@ -20127,7 +20126,7 @@
         <v>162</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E153" s="3">
         <v>2012</v>
@@ -20228,7 +20227,7 @@
         <v>162</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E154" s="3">
         <v>2012</v>
@@ -20329,7 +20328,7 @@
         <v>162</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E155" s="3">
         <v>2012</v>
@@ -20430,7 +20429,7 @@
         <v>162</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E156" s="3">
         <v>2012</v>
@@ -20531,7 +20530,7 @@
         <v>162</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E157" s="3">
         <v>2012</v>
@@ -20632,7 +20631,7 @@
         <v>162</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E158" s="3">
         <v>2012</v>
@@ -20834,7 +20833,7 @@
         <v>162</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E160" s="3">
         <v>2012</v>
@@ -20932,10 +20931,10 @@
         <v>97</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E161" s="3">
         <v>2012</v>
@@ -20944,10 +20943,10 @@
         <v>162</v>
       </c>
       <c r="G161" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="H161" s="8" t="s">
         <v>598</v>
-      </c>
-      <c r="H161" s="8" t="s">
-        <v>599</v>
       </c>
       <c r="I161" s="4">
         <v>1</v>
@@ -21036,7 +21035,7 @@
         <v>162</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E162" s="3">
         <v>2012</v>
@@ -21137,7 +21136,7 @@
         <v>162</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E163" s="3">
         <v>2012</v>
@@ -21238,7 +21237,7 @@
         <v>162</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E164" s="3">
         <v>2012</v>
@@ -21339,7 +21338,7 @@
         <v>162</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E165" s="3">
         <v>2011</v>
@@ -21440,7 +21439,7 @@
         <v>162</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E166" s="3">
         <v>2011</v>
@@ -21642,7 +21641,7 @@
         <v>162</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E168" s="3">
         <v>2011</v>
@@ -21743,7 +21742,7 @@
         <v>162</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E169" s="3">
         <v>2011</v>
@@ -21844,7 +21843,7 @@
         <v>162</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E170" s="3">
         <v>2011</v>
@@ -21945,7 +21944,7 @@
         <v>162</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E171" s="3">
         <v>2011</v>
@@ -22046,7 +22045,7 @@
         <v>162</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E172" s="3">
         <v>2011</v>
@@ -22147,7 +22146,7 @@
         <v>162</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E173" s="3">
         <v>2011</v>
@@ -22248,7 +22247,7 @@
         <v>162</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E174" s="3">
         <v>2011</v>
@@ -22450,7 +22449,7 @@
         <v>162</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E176" s="3">
         <v>2011</v>
@@ -22652,7 +22651,7 @@
         <v>162</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E178" s="3">
         <v>2010</v>
@@ -22854,7 +22853,7 @@
         <v>162</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E180" s="3">
         <v>2010</v>
@@ -22955,7 +22954,7 @@
         <v>162</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E181" s="3">
         <v>2010</v>
@@ -23056,7 +23055,7 @@
         <v>162</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E182" s="3">
         <v>2010</v>
@@ -23157,7 +23156,7 @@
         <v>162</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E183" s="3">
         <v>2010</v>
@@ -23258,7 +23257,7 @@
         <v>162</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E184" s="3">
         <v>2010</v>
@@ -23359,7 +23358,7 @@
         <v>162</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E185" s="3">
         <v>2010</v>
@@ -23460,7 +23459,7 @@
         <v>162</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E186" s="3">
         <v>2010</v>
@@ -23561,7 +23560,7 @@
         <v>162</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E187" s="3">
         <v>2010</v>
@@ -23763,7 +23762,7 @@
         <v>162</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E189" s="3">
         <v>2010</v>
@@ -23864,7 +23863,7 @@
         <v>162</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E190" s="3">
         <v>2010</v>
@@ -23965,7 +23964,7 @@
         <v>162</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E191" s="3">
         <v>2010</v>
@@ -24066,7 +24065,7 @@
         <v>162</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E192" s="3">
         <v>2009</v>
@@ -24369,7 +24368,7 @@
         <v>162</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E195" s="3">
         <v>2009</v>
@@ -24470,7 +24469,7 @@
         <v>162</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E196" s="3">
         <v>2009</v>
@@ -24571,7 +24570,7 @@
         <v>162</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E197" s="3">
         <v>2009</v>
@@ -24773,7 +24772,7 @@
         <v>162</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E199" s="3">
         <v>2009</v>
@@ -25076,7 +25075,7 @@
         <v>162</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E202" s="3">
         <v>2008</v>
@@ -25177,7 +25176,7 @@
         <v>162</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E203" s="3">
         <v>2008</v>
@@ -25278,7 +25277,7 @@
         <v>162</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E204" s="3">
         <v>2008</v>
@@ -25379,7 +25378,7 @@
         <v>162</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E205" s="3">
         <v>2008</v>
@@ -25480,7 +25479,7 @@
         <v>162</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E206" s="3">
         <v>2008</v>
@@ -25581,7 +25580,7 @@
         <v>162</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E207" s="3">
         <v>2008</v>
@@ -25679,10 +25678,10 @@
         <v>157</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E208" s="3">
         <v>2007</v>
@@ -25691,7 +25690,7 @@
         <v>162</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H208" s="4" t="s">
         <v>162</v>
@@ -25780,7 +25779,7 @@
         <v>156</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>398</v>
@@ -25792,10 +25791,10 @@
         <v>162</v>
       </c>
       <c r="G209" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="H209" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="H209" s="4" t="s">
-        <v>606</v>
       </c>
       <c r="I209" s="4">
         <v>1</v>
@@ -25880,11 +25879,11 @@
       <c r="B210" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C210" s="9" t="s">
-        <v>608</v>
+      <c r="C210" s="4" t="s">
+        <v>607</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E210" s="3">
         <v>2007</v>
@@ -25893,10 +25892,10 @@
         <v>162</v>
       </c>
       <c r="G210" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="H210" s="4" t="s">
         <v>600</v>
-      </c>
-      <c r="H210" s="4" t="s">
-        <v>601</v>
       </c>
       <c r="I210" s="4">
         <v>1</v>
@@ -25982,7 +25981,7 @@
         <v>159</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>400</v>
@@ -25991,13 +25990,13 @@
         <v>2006</v>
       </c>
       <c r="F211" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="G211" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="H211" s="4" t="s">
         <v>610</v>
-      </c>
-      <c r="G211" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="H211" s="4" t="s">
-        <v>611</v>
       </c>
       <c r="I211" s="4">
         <v>1</v>
@@ -26083,10 +26082,10 @@
         <v>158</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E212" s="3">
         <v>2006</v>
@@ -26095,7 +26094,7 @@
         <v>162</v>
       </c>
       <c r="G212" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H212" s="4" t="s">
         <v>162</v>
@@ -26184,7 +26183,7 @@
         <v>161</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>402</v>
@@ -26195,8 +26194,8 @@
       <c r="F213" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G213" s="9" t="s">
-        <v>617</v>
+      <c r="G213" s="4" t="s">
+        <v>616</v>
       </c>
       <c r="H213" s="4" t="s">
         <v>162</v>
@@ -26285,10 +26284,10 @@
         <v>160</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E214" s="3">
         <v>2005</v>
@@ -26297,7 +26296,7 @@
         <v>162</v>
       </c>
       <c r="G214" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H214" s="4" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
update to citation tags
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1424" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{406FAAD3-87D8-43FA-8CC3-DB5CAFA23C7C}"/>
+  <xr:revisionPtr revIDLastSave="1426" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCF88BB8-4416-F543-9DFF-0FBC32E43919}"/>
   <bookViews>
-    <workbookView xWindow="10430" yWindow="1050" windowWidth="36200" windowHeight="19690" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="1080" yWindow="820" windowWidth="43900" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1962,7 +1962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1987,9 +1987,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,9 +2009,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2052,7 +2049,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2158,7 +2155,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2300,7 +2297,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2314,7 +2311,7 @@
       <selection activeCell="E1" sqref="E1:AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
@@ -2344,7 +2341,7 @@
     <col min="28" max="28" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2444,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2475,7 +2472,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2489,7 +2486,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2503,7 +2500,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2517,7 +2514,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
@@ -2531,7 +2528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2545,7 +2542,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2559,7 +2556,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2573,7 +2570,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2587,7 +2584,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2598,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2615,7 +2612,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2626,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2643,7 +2640,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2654,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2671,7 +2668,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2685,7 +2682,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +2696,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2713,7 +2710,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2724,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2738,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2755,7 +2752,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2769,7 +2766,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +2780,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2825,7 +2822,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2839,7 +2836,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2853,7 +2850,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2867,7 +2864,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2881,7 +2878,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2895,7 +2892,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2923,7 +2920,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -2937,7 +2934,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -2951,7 +2948,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -2979,7 +2976,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -2993,7 +2990,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -3007,7 +3004,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -3035,7 +3032,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -3049,7 +3046,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -3063,7 +3060,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -3077,7 +3074,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -3091,7 +3088,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -3105,7 +3102,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -3119,7 +3116,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -3133,7 +3130,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -3147,7 +3144,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -3161,7 +3158,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -3175,7 +3172,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -3189,7 +3186,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -3203,7 +3200,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -3231,7 +3228,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -3245,7 +3242,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -3259,7 +3256,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -3273,7 +3270,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -3287,7 +3284,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -3301,7 +3298,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -3315,7 +3312,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -3329,7 +3326,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -3343,7 +3340,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -3371,7 +3368,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -3385,7 +3382,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -3399,7 +3396,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -3413,7 +3410,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -3427,7 +3424,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
@@ -3455,7 +3452,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -3469,7 +3466,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -3483,7 +3480,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>152</v>
       </c>
@@ -3497,7 +3494,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
@@ -3511,7 +3508,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>74</v>
       </c>
@@ -3525,7 +3522,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>75</v>
       </c>
@@ -3539,7 +3536,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>76</v>
       </c>
@@ -3553,7 +3550,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>77</v>
       </c>
@@ -3567,7 +3564,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
@@ -3581,7 +3578,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>79</v>
       </c>
@@ -3595,7 +3592,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -3609,7 +3606,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>81</v>
       </c>
@@ -3623,7 +3620,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>82</v>
       </c>
@@ -3637,7 +3634,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>83</v>
       </c>
@@ -3651,7 +3648,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>84</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -3679,7 +3676,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>86</v>
       </c>
@@ -3693,7 +3690,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>87</v>
       </c>
@@ -3707,7 +3704,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>88</v>
       </c>
@@ -3721,7 +3718,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>89</v>
       </c>
@@ -3735,7 +3732,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
@@ -3749,7 +3746,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>91</v>
       </c>
@@ -3763,7 +3760,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
@@ -3777,7 +3774,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>93</v>
       </c>
@@ -3791,7 +3788,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>94</v>
       </c>
@@ -3805,7 +3802,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -3819,7 +3816,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>96</v>
       </c>
@@ -3833,7 +3830,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>97</v>
       </c>
@@ -3847,7 +3844,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>98</v>
       </c>
@@ -3861,7 +3858,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>153</v>
       </c>
@@ -3875,7 +3872,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>99</v>
       </c>
@@ -3889,7 +3886,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>100</v>
       </c>
@@ -3903,7 +3900,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>101</v>
       </c>
@@ -3917,7 +3914,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>102</v>
       </c>
@@ -3931,7 +3928,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>103</v>
       </c>
@@ -3945,7 +3942,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>104</v>
       </c>
@@ -3959,7 +3956,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>105</v>
       </c>
@@ -3973,7 +3970,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>106</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>107</v>
       </c>
@@ -4001,7 +3998,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>108</v>
       </c>
@@ -4015,7 +4012,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>109</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>110</v>
       </c>
@@ -4043,7 +4040,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>111</v>
       </c>
@@ -4057,7 +4054,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>112</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>113</v>
       </c>
@@ -4085,7 +4082,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>114</v>
       </c>
@@ -4099,7 +4096,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>115</v>
       </c>
@@ -4113,7 +4110,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>116</v>
       </c>
@@ -4127,7 +4124,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>154</v>
       </c>
@@ -4155,7 +4152,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>118</v>
       </c>
@@ -4169,7 +4166,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>119</v>
       </c>
@@ -4183,7 +4180,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>120</v>
       </c>
@@ -4197,7 +4194,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>121</v>
       </c>
@@ -4211,7 +4208,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>122</v>
       </c>
@@ -4225,7 +4222,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>123</v>
       </c>
@@ -4239,7 +4236,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>124</v>
       </c>
@@ -4253,7 +4250,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>125</v>
       </c>
@@ -4267,7 +4264,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>126</v>
       </c>
@@ -4281,7 +4278,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>127</v>
       </c>
@@ -4295,7 +4292,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>128</v>
       </c>
@@ -4309,7 +4306,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>129</v>
       </c>
@@ -4323,7 +4320,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>130</v>
       </c>
@@ -4337,7 +4334,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>131</v>
       </c>
@@ -4351,7 +4348,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>132</v>
       </c>
@@ -4365,7 +4362,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>133</v>
       </c>
@@ -4379,7 +4376,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>134</v>
       </c>
@@ -4393,7 +4390,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>135</v>
       </c>
@@ -4407,7 +4404,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>136</v>
       </c>
@@ -4421,7 +4418,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>137</v>
       </c>
@@ -4435,7 +4432,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>138</v>
       </c>
@@ -4449,7 +4446,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>139</v>
       </c>
@@ -4463,7 +4460,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>140</v>
       </c>
@@ -4477,7 +4474,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>141</v>
       </c>
@@ -4491,7 +4488,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>142</v>
       </c>
@@ -4505,7 +4502,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>143</v>
       </c>
@@ -4519,7 +4516,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>144</v>
       </c>
@@ -4533,7 +4530,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>145</v>
       </c>
@@ -4547,7 +4544,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>146</v>
       </c>
@@ -4561,7 +4558,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>147</v>
       </c>
@@ -4575,7 +4572,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>148</v>
       </c>
@@ -4589,7 +4586,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>149</v>
       </c>
@@ -4603,7 +4600,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>150</v>
       </c>
@@ -4617,7 +4614,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -4631,7 +4628,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>155</v>
       </c>
@@ -4645,7 +4642,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>156</v>
       </c>
@@ -4659,7 +4656,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>158</v>
       </c>
@@ -4673,7 +4670,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>159</v>
       </c>
@@ -4687,7 +4684,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>160</v>
       </c>
@@ -4701,7 +4698,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>161</v>
       </c>
@@ -4728,16 +4725,16 @@
   </sheetPr>
   <dimension ref="A1:AG213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="210.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" style="1" customWidth="1"/>
@@ -4768,7 +4765,7 @@
     <col min="33" max="33" width="6.1640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>188</v>
       </c>
@@ -4869,7 +4866,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>38229171</v>
       </c>
@@ -4970,7 +4967,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>37689782</v>
       </c>
@@ -5071,7 +5068,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>37171501</v>
       </c>
@@ -5172,7 +5169,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>37165871</v>
       </c>
@@ -5273,7 +5270,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>36214830</v>
       </c>
@@ -5374,7 +5371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>36581621</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>36376295</v>
       </c>
@@ -5576,7 +5573,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>35894642</v>
       </c>
@@ -5677,7 +5674,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>35166671</v>
       </c>
@@ -5778,7 +5775,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>22495311</v>
       </c>
@@ -5879,7 +5876,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>37546828</v>
       </c>
@@ -5980,7 +5977,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>37418489</v>
       </c>
@@ -6081,7 +6078,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>162</v>
       </c>
@@ -6182,7 +6179,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>162</v>
       </c>
@@ -6283,7 +6280,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>37205500</v>
       </c>
@@ -6384,7 +6381,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>162</v>
       </c>
@@ -6485,7 +6482,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>162</v>
       </c>
@@ -6586,7 +6583,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>36229773</v>
       </c>
@@ -6687,7 +6684,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>162</v>
       </c>
@@ -6788,7 +6785,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>35666730</v>
       </c>
@@ -6889,7 +6886,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>35285134</v>
       </c>
@@ -6990,7 +6987,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>35129650</v>
       </c>
@@ -7091,7 +7088,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>35482673</v>
       </c>
@@ -7192,7 +7189,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>35653334</v>
       </c>
@@ -7293,7 +7290,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>35654975</v>
       </c>
@@ -7394,7 +7391,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>35710981</v>
       </c>
@@ -7495,7 +7492,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>35915156</v>
       </c>
@@ -7596,7 +7593,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>35186008</v>
       </c>
@@ -7697,7 +7694,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>35848019</v>
       </c>
@@ -7798,7 +7795,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>35705896</v>
       </c>
@@ -7899,7 +7896,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>162</v>
       </c>
@@ -8000,7 +7997,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>33541420</v>
       </c>
@@ -8101,7 +8098,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>162</v>
       </c>
@@ -8202,7 +8199,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>162</v>
       </c>
@@ -8303,7 +8300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>162</v>
       </c>
@@ -8404,7 +8401,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>34426578</v>
       </c>
@@ -8505,7 +8502,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>162</v>
       </c>
@@ -8606,7 +8603,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>34184541</v>
       </c>
@@ -8707,7 +8704,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>34547901</v>
       </c>
@@ -8808,7 +8805,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>162</v>
       </c>
@@ -8909,7 +8906,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>162</v>
       </c>
@@ -9010,7 +9007,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>34140684</v>
       </c>
@@ -9111,7 +9108,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>33853351</v>
       </c>
@@ -9212,7 +9209,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>34799566</v>
       </c>
@@ -9313,7 +9310,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>32306029</v>
       </c>
@@ -9414,7 +9411,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>162</v>
       </c>
@@ -9515,7 +9512,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>162</v>
       </c>
@@ -9616,7 +9613,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>33972514</v>
       </c>
@@ -9717,7 +9714,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>33464320</v>
       </c>
@@ -9818,7 +9815,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>33397451</v>
       </c>
@@ -9919,7 +9916,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>33561241</v>
       </c>
@@ -10020,7 +10017,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>34385711</v>
       </c>
@@ -10121,7 +10118,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>162</v>
       </c>
@@ -10222,7 +10219,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>34139859</v>
       </c>
@@ -10323,7 +10320,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="56" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>162</v>
       </c>
@@ -10424,7 +10421,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>162</v>
       </c>
@@ -10525,7 +10522,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>33321069</v>
       </c>
@@ -10626,7 +10623,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>32600345</v>
       </c>
@@ -10727,7 +10724,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>32915777</v>
       </c>
@@ -10828,7 +10825,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>162</v>
       </c>
@@ -10929,7 +10926,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>162</v>
       </c>
@@ -11030,7 +11027,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>162</v>
       </c>
@@ -11131,7 +11128,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>32282858</v>
       </c>
@@ -11232,7 +11229,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>32011695</v>
       </c>
@@ -11333,7 +11330,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>162</v>
       </c>
@@ -11434,7 +11431,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>32541925</v>
       </c>
@@ -11535,7 +11532,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>32833022</v>
       </c>
@@ -11636,7 +11633,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>31843946</v>
       </c>
@@ -11737,7 +11734,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>162</v>
       </c>
@@ -11838,7 +11835,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>32340472</v>
       </c>
@@ -11939,7 +11936,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="72" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>33031386</v>
       </c>
@@ -12040,7 +12037,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>162</v>
       </c>
@@ -12141,7 +12138,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>162</v>
       </c>
@@ -12242,7 +12239,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>162</v>
       </c>
@@ -12343,7 +12340,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>32408895</v>
       </c>
@@ -12444,7 +12441,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>32705316</v>
       </c>
@@ -12545,7 +12542,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>32841307</v>
       </c>
@@ -12646,7 +12643,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>162</v>
       </c>
@@ -12747,7 +12744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>30616593</v>
       </c>
@@ -12848,7 +12845,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>162</v>
       </c>
@@ -12949,7 +12946,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
@@ -13050,7 +13047,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>162</v>
       </c>
@@ -13151,7 +13148,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>162</v>
       </c>
@@ -13252,7 +13249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>31659023</v>
       </c>
@@ -13353,7 +13350,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>30711642</v>
       </c>
@@ -13454,7 +13451,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>31173123</v>
       </c>
@@ -13555,7 +13552,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>30753705</v>
       </c>
@@ -13656,7 +13653,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
@@ -13757,7 +13754,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>162</v>
       </c>
@@ -13858,7 +13855,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>29880058</v>
       </c>
@@ -13959,7 +13956,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
@@ -14060,7 +14057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>29459708</v>
       </c>
@@ -14161,7 +14158,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>162</v>
       </c>
@@ -14262,7 +14259,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>30525989</v>
       </c>
@@ -14363,7 +14360,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>30254083</v>
       </c>
@@ -14464,7 +14461,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>29068475</v>
       </c>
@@ -14565,7 +14562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>29987113</v>
       </c>
@@ -14666,7 +14663,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>162</v>
       </c>
@@ -14767,7 +14764,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>28566273</v>
       </c>
@@ -14868,7 +14865,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>29257133</v>
       </c>
@@ -14969,7 +14966,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>28193182</v>
       </c>
@@ -15070,7 +15067,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>162</v>
       </c>
@@ -15171,7 +15168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="104" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>28981714</v>
       </c>
@@ -15272,7 +15269,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="105" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>28559929</v>
       </c>
@@ -15373,7 +15370,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>28869590</v>
       </c>
@@ -15474,7 +15471,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>28285767</v>
       </c>
@@ -15575,7 +15572,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="108" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>162</v>
       </c>
@@ -15676,7 +15673,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="109" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>28438156</v>
       </c>
@@ -15777,7 +15774,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="110" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>28025330</v>
       </c>
@@ -15878,7 +15875,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>27702834</v>
       </c>
@@ -15979,7 +15976,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>28459453</v>
       </c>
@@ -16080,7 +16077,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>162</v>
       </c>
@@ -16181,7 +16178,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="114" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>26878723</v>
       </c>
@@ -16282,7 +16279,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="115" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>27616605</v>
       </c>
@@ -16383,7 +16380,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>26821629</v>
       </c>
@@ -16484,7 +16481,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="117" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>162</v>
       </c>
@@ -16585,7 +16582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="118" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>27487162</v>
       </c>
@@ -16686,7 +16683,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="119" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>26708677</v>
       </c>
@@ -16787,7 +16784,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="120" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>27340225</v>
       </c>
@@ -16888,7 +16885,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>27398621</v>
       </c>
@@ -16989,7 +16986,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="122" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>27618452</v>
       </c>
@@ -17090,7 +17087,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="123" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>27879406</v>
       </c>
@@ -17191,7 +17188,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="124" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>26140591</v>
       </c>
@@ -17292,7 +17289,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="125" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>26551672</v>
       </c>
@@ -17393,7 +17390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="126" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>26074316</v>
       </c>
@@ -17494,7 +17491,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>25388149</v>
       </c>
@@ -17595,7 +17592,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="128" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>24699409</v>
       </c>
@@ -17696,7 +17693,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>162</v>
       </c>
@@ -17797,7 +17794,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="130" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>24509480</v>
       </c>
@@ -17898,7 +17895,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>24759409</v>
       </c>
@@ -17999,7 +17996,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="132" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>24584071</v>
       </c>
@@ -18100,7 +18097,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>25165093</v>
       </c>
@@ -18201,7 +18198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="134" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>24981077</v>
       </c>
@@ -18302,7 +18299,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>162</v>
       </c>
@@ -18403,7 +18400,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="136" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>162</v>
       </c>
@@ -18504,7 +18501,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>24097064</v>
       </c>
@@ -18605,7 +18602,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>24097068</v>
       </c>
@@ -18706,7 +18703,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="139" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>162</v>
       </c>
@@ -18807,7 +18804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="140" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>23675308</v>
       </c>
@@ -18908,7 +18905,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>162</v>
       </c>
@@ -19009,7 +19006,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="142" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>23202125</v>
       </c>
@@ -19110,7 +19107,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="143" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>162</v>
       </c>
@@ -19211,7 +19208,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="144" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>162</v>
       </c>
@@ -19312,7 +19309,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="145" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>162</v>
       </c>
@@ -19413,7 +19410,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="146" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>22581228</v>
       </c>
@@ -19514,7 +19511,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="147" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>22238593</v>
       </c>
@@ -19615,7 +19612,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>22556366</v>
       </c>
@@ -19716,7 +19713,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="149" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>22446960</v>
       </c>
@@ -19817,7 +19814,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="150" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>22539988</v>
       </c>
@@ -19918,7 +19915,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>23041452</v>
       </c>
@@ -20019,7 +20016,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="152" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>23152477</v>
       </c>
@@ -20120,7 +20117,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>22698912</v>
       </c>
@@ -20221,7 +20218,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="154" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>23144628</v>
       </c>
@@ -20322,7 +20319,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="155" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>22885924</v>
       </c>
@@ -20423,7 +20420,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>22885922</v>
       </c>
@@ -20524,7 +20521,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>22325160</v>
       </c>
@@ -20625,7 +20622,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>22544366</v>
       </c>
@@ -20726,7 +20723,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>22479202</v>
       </c>
@@ -20827,7 +20824,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>22607825</v>
       </c>
@@ -20849,7 +20846,7 @@
       <c r="G160" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="H160" s="10" t="s">
+      <c r="H160" s="3" t="s">
         <v>594</v>
       </c>
       <c r="I160" s="8">
@@ -20928,7 +20925,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>22264825</v>
       </c>
@@ -21029,7 +21026,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="162" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>22693455</v>
       </c>
@@ -21130,7 +21127,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>22876189</v>
       </c>
@@ -21231,7 +21228,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>21606135</v>
       </c>
@@ -21332,7 +21329,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>21597005</v>
       </c>
@@ -21433,7 +21430,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="166" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>162</v>
       </c>
@@ -21534,7 +21531,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>21909115</v>
       </c>
@@ -21635,7 +21632,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="168" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>21423719</v>
       </c>
@@ -21736,7 +21733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="169" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>21873549</v>
       </c>
@@ -21837,7 +21834,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="170" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>22144573</v>
       </c>
@@ -21938,7 +21935,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="171" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>21909110</v>
       </c>
@@ -22039,7 +22036,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="172" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>21757122</v>
       </c>
@@ -22140,7 +22137,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="173" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>21378990</v>
       </c>
@@ -22241,7 +22238,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="174" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>21852963</v>
       </c>
@@ -22342,7 +22339,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="175" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>21308769</v>
       </c>
@@ -22443,7 +22440,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="176" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>21408211</v>
       </c>
@@ -22544,7 +22541,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="177" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>20935630</v>
       </c>
@@ -22645,7 +22642,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="178" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>20686565</v>
       </c>
@@ -22746,7 +22743,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>20858683</v>
       </c>
@@ -22847,7 +22844,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="180" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>20923989</v>
       </c>
@@ -22948,7 +22945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="181" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>20657596</v>
       </c>
@@ -23049,7 +23046,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="182" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>20081857</v>
       </c>
@@ -23150,7 +23147,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="183" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>20418890</v>
       </c>
@@ -23251,7 +23248,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="184" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>20881960</v>
       </c>
@@ -23352,7 +23349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="185" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>20933357</v>
       </c>
@@ -23453,7 +23450,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="186" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>20935629</v>
       </c>
@@ -23554,7 +23551,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="187" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>20838612</v>
       </c>
@@ -23655,7 +23652,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="188" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>20081858</v>
       </c>
@@ -23756,7 +23753,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="189" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>20648472</v>
       </c>
@@ -23857,7 +23854,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="190" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>20581827</v>
       </c>
@@ -23958,7 +23955,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>19820697</v>
       </c>
@@ -24059,7 +24056,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="192" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>19553259</v>
       </c>
@@ -24160,7 +24157,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="193" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>19060906</v>
       </c>
@@ -24261,7 +24258,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="194" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>19198609</v>
       </c>
@@ -24362,7 +24359,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="195" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>19430483</v>
       </c>
@@ -24463,7 +24460,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="196" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>19389826</v>
       </c>
@@ -24564,7 +24561,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="197" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>19198612</v>
       </c>
@@ -24665,7 +24662,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="198" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>19377085</v>
       </c>
@@ -24766,7 +24763,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="199" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>19602701</v>
       </c>
@@ -24867,7 +24864,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="200" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>19060907</v>
       </c>
@@ -24968,7 +24965,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="201" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>18678614</v>
       </c>
@@ -25069,7 +25066,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="202" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>18454148</v>
       </c>
@@ -25170,7 +25167,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="203" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>18391950</v>
       </c>
@@ -25271,7 +25268,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="204" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>18372903</v>
       </c>
@@ -25372,7 +25369,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="205" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>18852200</v>
       </c>
@@ -25473,7 +25470,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="206" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>18193044</v>
       </c>
@@ -25574,7 +25571,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="207" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>17767157</v>
       </c>
@@ -25675,7 +25672,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="208" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>17159977</v>
       </c>
@@ -25776,7 +25773,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="209" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>17463246</v>
       </c>
@@ -25877,7 +25874,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="210" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>16494531</v>
       </c>
@@ -25978,7 +25975,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="211" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>16680197</v>
       </c>
@@ -26079,7 +26076,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="212" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>16151517</v>
       </c>
@@ -26180,7 +26177,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="213" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>16352722</v>
       </c>
@@ -26293,7 +26290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@958b0b7e16b62950415b1db9076bbdcb9dbae23f 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1424" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{406FAAD3-87D8-43FA-8CC3-DB5CAFA23C7C}"/>
+  <xr:revisionPtr revIDLastSave="1426" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCF88BB8-4416-F543-9DFF-0FBC32E43919}"/>
   <bookViews>
-    <workbookView xWindow="10430" yWindow="1050" windowWidth="36200" windowHeight="19690" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="1080" yWindow="820" windowWidth="43900" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1962,7 +1962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1987,9 +1987,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,9 +2009,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2052,7 +2049,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2158,7 +2155,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2300,7 +2297,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2314,7 +2311,7 @@
       <selection activeCell="E1" sqref="E1:AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
@@ -2344,7 +2341,7 @@
     <col min="28" max="28" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2444,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2475,7 +2472,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2489,7 +2486,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2503,7 +2500,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2517,7 +2514,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
@@ -2531,7 +2528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2545,7 +2542,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2559,7 +2556,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2573,7 +2570,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2587,7 +2584,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2598,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2615,7 +2612,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2626,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2643,7 +2640,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2654,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2671,7 +2668,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2685,7 +2682,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +2696,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2713,7 +2710,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2724,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2738,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2755,7 +2752,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2769,7 +2766,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +2780,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2825,7 +2822,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2839,7 +2836,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2853,7 +2850,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2867,7 +2864,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2881,7 +2878,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2895,7 +2892,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2923,7 +2920,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -2937,7 +2934,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -2951,7 +2948,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -2979,7 +2976,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -2993,7 +2990,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -3007,7 +3004,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -3035,7 +3032,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -3049,7 +3046,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -3063,7 +3060,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -3077,7 +3074,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -3091,7 +3088,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -3105,7 +3102,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -3119,7 +3116,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -3133,7 +3130,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -3147,7 +3144,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -3161,7 +3158,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -3175,7 +3172,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -3189,7 +3186,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -3203,7 +3200,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -3231,7 +3228,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -3245,7 +3242,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -3259,7 +3256,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -3273,7 +3270,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -3287,7 +3284,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -3301,7 +3298,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -3315,7 +3312,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -3329,7 +3326,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -3343,7 +3340,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -3371,7 +3368,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -3385,7 +3382,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -3399,7 +3396,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -3413,7 +3410,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -3427,7 +3424,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
@@ -3455,7 +3452,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -3469,7 +3466,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -3483,7 +3480,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>152</v>
       </c>
@@ -3497,7 +3494,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
@@ -3511,7 +3508,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>74</v>
       </c>
@@ -3525,7 +3522,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>75</v>
       </c>
@@ -3539,7 +3536,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>76</v>
       </c>
@@ -3553,7 +3550,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>77</v>
       </c>
@@ -3567,7 +3564,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
@@ -3581,7 +3578,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>79</v>
       </c>
@@ -3595,7 +3592,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -3609,7 +3606,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>81</v>
       </c>
@@ -3623,7 +3620,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>82</v>
       </c>
@@ -3637,7 +3634,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>83</v>
       </c>
@@ -3651,7 +3648,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>84</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -3679,7 +3676,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>86</v>
       </c>
@@ -3693,7 +3690,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>87</v>
       </c>
@@ -3707,7 +3704,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>88</v>
       </c>
@@ -3721,7 +3718,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>89</v>
       </c>
@@ -3735,7 +3732,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
@@ -3749,7 +3746,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>91</v>
       </c>
@@ -3763,7 +3760,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
@@ -3777,7 +3774,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>93</v>
       </c>
@@ -3791,7 +3788,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>94</v>
       </c>
@@ -3805,7 +3802,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -3819,7 +3816,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>96</v>
       </c>
@@ -3833,7 +3830,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>97</v>
       </c>
@@ -3847,7 +3844,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>98</v>
       </c>
@@ -3861,7 +3858,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>153</v>
       </c>
@@ -3875,7 +3872,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>99</v>
       </c>
@@ -3889,7 +3886,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>100</v>
       </c>
@@ -3903,7 +3900,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>101</v>
       </c>
@@ -3917,7 +3914,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>102</v>
       </c>
@@ -3931,7 +3928,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>103</v>
       </c>
@@ -3945,7 +3942,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>104</v>
       </c>
@@ -3959,7 +3956,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>105</v>
       </c>
@@ -3973,7 +3970,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>106</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>107</v>
       </c>
@@ -4001,7 +3998,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>108</v>
       </c>
@@ -4015,7 +4012,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>109</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>110</v>
       </c>
@@ -4043,7 +4040,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>111</v>
       </c>
@@ -4057,7 +4054,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>112</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>113</v>
       </c>
@@ -4085,7 +4082,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>114</v>
       </c>
@@ -4099,7 +4096,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>115</v>
       </c>
@@ -4113,7 +4110,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>116</v>
       </c>
@@ -4127,7 +4124,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>154</v>
       </c>
@@ -4155,7 +4152,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>118</v>
       </c>
@@ -4169,7 +4166,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>119</v>
       </c>
@@ -4183,7 +4180,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>120</v>
       </c>
@@ -4197,7 +4194,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>121</v>
       </c>
@@ -4211,7 +4208,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>122</v>
       </c>
@@ -4225,7 +4222,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>123</v>
       </c>
@@ -4239,7 +4236,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>124</v>
       </c>
@@ -4253,7 +4250,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>125</v>
       </c>
@@ -4267,7 +4264,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>126</v>
       </c>
@@ -4281,7 +4278,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>127</v>
       </c>
@@ -4295,7 +4292,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>128</v>
       </c>
@@ -4309,7 +4306,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>129</v>
       </c>
@@ -4323,7 +4320,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>130</v>
       </c>
@@ -4337,7 +4334,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>131</v>
       </c>
@@ -4351,7 +4348,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>132</v>
       </c>
@@ -4365,7 +4362,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>133</v>
       </c>
@@ -4379,7 +4376,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>134</v>
       </c>
@@ -4393,7 +4390,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>135</v>
       </c>
@@ -4407,7 +4404,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>136</v>
       </c>
@@ -4421,7 +4418,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>137</v>
       </c>
@@ -4435,7 +4432,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>138</v>
       </c>
@@ -4449,7 +4446,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>139</v>
       </c>
@@ -4463,7 +4460,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>140</v>
       </c>
@@ -4477,7 +4474,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>141</v>
       </c>
@@ -4491,7 +4488,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>142</v>
       </c>
@@ -4505,7 +4502,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>143</v>
       </c>
@@ -4519,7 +4516,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>144</v>
       </c>
@@ -4533,7 +4530,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>145</v>
       </c>
@@ -4547,7 +4544,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>146</v>
       </c>
@@ -4561,7 +4558,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>147</v>
       </c>
@@ -4575,7 +4572,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>148</v>
       </c>
@@ -4589,7 +4586,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>149</v>
       </c>
@@ -4603,7 +4600,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>150</v>
       </c>
@@ -4617,7 +4614,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -4631,7 +4628,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>155</v>
       </c>
@@ -4645,7 +4642,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>156</v>
       </c>
@@ -4659,7 +4656,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>158</v>
       </c>
@@ -4673,7 +4670,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>159</v>
       </c>
@@ -4687,7 +4684,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>160</v>
       </c>
@@ -4701,7 +4698,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>161</v>
       </c>
@@ -4728,16 +4725,16 @@
   </sheetPr>
   <dimension ref="A1:AG213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="210.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" style="1" customWidth="1"/>
@@ -4768,7 +4765,7 @@
     <col min="33" max="33" width="6.1640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>188</v>
       </c>
@@ -4869,7 +4866,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>38229171</v>
       </c>
@@ -4970,7 +4967,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>37689782</v>
       </c>
@@ -5071,7 +5068,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>37171501</v>
       </c>
@@ -5172,7 +5169,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>37165871</v>
       </c>
@@ -5273,7 +5270,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>36214830</v>
       </c>
@@ -5374,7 +5371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>36581621</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>36376295</v>
       </c>
@@ -5576,7 +5573,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>35894642</v>
       </c>
@@ -5677,7 +5674,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>35166671</v>
       </c>
@@ -5778,7 +5775,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>22495311</v>
       </c>
@@ -5879,7 +5876,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>37546828</v>
       </c>
@@ -5980,7 +5977,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>37418489</v>
       </c>
@@ -6081,7 +6078,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>162</v>
       </c>
@@ -6182,7 +6179,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>162</v>
       </c>
@@ -6283,7 +6280,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>37205500</v>
       </c>
@@ -6384,7 +6381,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>162</v>
       </c>
@@ -6485,7 +6482,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>162</v>
       </c>
@@ -6586,7 +6583,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>36229773</v>
       </c>
@@ -6687,7 +6684,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>162</v>
       </c>
@@ -6788,7 +6785,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>35666730</v>
       </c>
@@ -6889,7 +6886,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>35285134</v>
       </c>
@@ -6990,7 +6987,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>35129650</v>
       </c>
@@ -7091,7 +7088,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>35482673</v>
       </c>
@@ -7192,7 +7189,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>35653334</v>
       </c>
@@ -7293,7 +7290,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>35654975</v>
       </c>
@@ -7394,7 +7391,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>35710981</v>
       </c>
@@ -7495,7 +7492,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>35915156</v>
       </c>
@@ -7596,7 +7593,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>35186008</v>
       </c>
@@ -7697,7 +7694,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>35848019</v>
       </c>
@@ -7798,7 +7795,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>35705896</v>
       </c>
@@ -7899,7 +7896,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>162</v>
       </c>
@@ -8000,7 +7997,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>33541420</v>
       </c>
@@ -8101,7 +8098,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>162</v>
       </c>
@@ -8202,7 +8199,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>162</v>
       </c>
@@ -8303,7 +8300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>162</v>
       </c>
@@ -8404,7 +8401,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>34426578</v>
       </c>
@@ -8505,7 +8502,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>162</v>
       </c>
@@ -8606,7 +8603,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>34184541</v>
       </c>
@@ -8707,7 +8704,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>34547901</v>
       </c>
@@ -8808,7 +8805,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>162</v>
       </c>
@@ -8909,7 +8906,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>162</v>
       </c>
@@ -9010,7 +9007,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>34140684</v>
       </c>
@@ -9111,7 +9108,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>33853351</v>
       </c>
@@ -9212,7 +9209,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>34799566</v>
       </c>
@@ -9313,7 +9310,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>32306029</v>
       </c>
@@ -9414,7 +9411,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>162</v>
       </c>
@@ -9515,7 +9512,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>162</v>
       </c>
@@ -9616,7 +9613,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>33972514</v>
       </c>
@@ -9717,7 +9714,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>33464320</v>
       </c>
@@ -9818,7 +9815,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>33397451</v>
       </c>
@@ -9919,7 +9916,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>33561241</v>
       </c>
@@ -10020,7 +10017,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>34385711</v>
       </c>
@@ -10121,7 +10118,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>162</v>
       </c>
@@ -10222,7 +10219,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>34139859</v>
       </c>
@@ -10323,7 +10320,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="56" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>162</v>
       </c>
@@ -10424,7 +10421,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>162</v>
       </c>
@@ -10525,7 +10522,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>33321069</v>
       </c>
@@ -10626,7 +10623,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>32600345</v>
       </c>
@@ -10727,7 +10724,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>32915777</v>
       </c>
@@ -10828,7 +10825,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>162</v>
       </c>
@@ -10929,7 +10926,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>162</v>
       </c>
@@ -11030,7 +11027,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>162</v>
       </c>
@@ -11131,7 +11128,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>32282858</v>
       </c>
@@ -11232,7 +11229,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>32011695</v>
       </c>
@@ -11333,7 +11330,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>162</v>
       </c>
@@ -11434,7 +11431,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>32541925</v>
       </c>
@@ -11535,7 +11532,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>32833022</v>
       </c>
@@ -11636,7 +11633,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>31843946</v>
       </c>
@@ -11737,7 +11734,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>162</v>
       </c>
@@ -11838,7 +11835,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>32340472</v>
       </c>
@@ -11939,7 +11936,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="72" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>33031386</v>
       </c>
@@ -12040,7 +12037,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>162</v>
       </c>
@@ -12141,7 +12138,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>162</v>
       </c>
@@ -12242,7 +12239,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>162</v>
       </c>
@@ -12343,7 +12340,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>32408895</v>
       </c>
@@ -12444,7 +12441,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>32705316</v>
       </c>
@@ -12545,7 +12542,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>32841307</v>
       </c>
@@ -12646,7 +12643,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>162</v>
       </c>
@@ -12747,7 +12744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>30616593</v>
       </c>
@@ -12848,7 +12845,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>162</v>
       </c>
@@ -12949,7 +12946,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
@@ -13050,7 +13047,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>162</v>
       </c>
@@ -13151,7 +13148,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>162</v>
       </c>
@@ -13252,7 +13249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>31659023</v>
       </c>
@@ -13353,7 +13350,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>30711642</v>
       </c>
@@ -13454,7 +13451,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>31173123</v>
       </c>
@@ -13555,7 +13552,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>30753705</v>
       </c>
@@ -13656,7 +13653,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
@@ -13757,7 +13754,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>162</v>
       </c>
@@ -13858,7 +13855,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>29880058</v>
       </c>
@@ -13959,7 +13956,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
@@ -14060,7 +14057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>29459708</v>
       </c>
@@ -14161,7 +14158,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>162</v>
       </c>
@@ -14262,7 +14259,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>30525989</v>
       </c>
@@ -14363,7 +14360,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>30254083</v>
       </c>
@@ -14464,7 +14461,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>29068475</v>
       </c>
@@ -14565,7 +14562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>29987113</v>
       </c>
@@ -14666,7 +14663,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>162</v>
       </c>
@@ -14767,7 +14764,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>28566273</v>
       </c>
@@ -14868,7 +14865,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>29257133</v>
       </c>
@@ -14969,7 +14966,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>28193182</v>
       </c>
@@ -15070,7 +15067,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>162</v>
       </c>
@@ -15171,7 +15168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="104" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>28981714</v>
       </c>
@@ -15272,7 +15269,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="105" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>28559929</v>
       </c>
@@ -15373,7 +15370,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>28869590</v>
       </c>
@@ -15474,7 +15471,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>28285767</v>
       </c>
@@ -15575,7 +15572,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="108" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>162</v>
       </c>
@@ -15676,7 +15673,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="109" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>28438156</v>
       </c>
@@ -15777,7 +15774,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="110" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>28025330</v>
       </c>
@@ -15878,7 +15875,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>27702834</v>
       </c>
@@ -15979,7 +15976,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>28459453</v>
       </c>
@@ -16080,7 +16077,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>162</v>
       </c>
@@ -16181,7 +16178,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="114" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>26878723</v>
       </c>
@@ -16282,7 +16279,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="115" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>27616605</v>
       </c>
@@ -16383,7 +16380,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>26821629</v>
       </c>
@@ -16484,7 +16481,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="117" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>162</v>
       </c>
@@ -16585,7 +16582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="118" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>27487162</v>
       </c>
@@ -16686,7 +16683,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="119" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>26708677</v>
       </c>
@@ -16787,7 +16784,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="120" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>27340225</v>
       </c>
@@ -16888,7 +16885,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>27398621</v>
       </c>
@@ -16989,7 +16986,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="122" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>27618452</v>
       </c>
@@ -17090,7 +17087,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="123" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>27879406</v>
       </c>
@@ -17191,7 +17188,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="124" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>26140591</v>
       </c>
@@ -17292,7 +17289,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="125" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>26551672</v>
       </c>
@@ -17393,7 +17390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="126" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>26074316</v>
       </c>
@@ -17494,7 +17491,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>25388149</v>
       </c>
@@ -17595,7 +17592,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="128" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>24699409</v>
       </c>
@@ -17696,7 +17693,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>162</v>
       </c>
@@ -17797,7 +17794,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="130" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>24509480</v>
       </c>
@@ -17898,7 +17895,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>24759409</v>
       </c>
@@ -17999,7 +17996,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="132" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>24584071</v>
       </c>
@@ -18100,7 +18097,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>25165093</v>
       </c>
@@ -18201,7 +18198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="134" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>24981077</v>
       </c>
@@ -18302,7 +18299,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>162</v>
       </c>
@@ -18403,7 +18400,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="136" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>162</v>
       </c>
@@ -18504,7 +18501,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>24097064</v>
       </c>
@@ -18605,7 +18602,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>24097068</v>
       </c>
@@ -18706,7 +18703,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="139" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>162</v>
       </c>
@@ -18807,7 +18804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="140" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>23675308</v>
       </c>
@@ -18908,7 +18905,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>162</v>
       </c>
@@ -19009,7 +19006,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="142" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>23202125</v>
       </c>
@@ -19110,7 +19107,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="143" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>162</v>
       </c>
@@ -19211,7 +19208,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="144" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>162</v>
       </c>
@@ -19312,7 +19309,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="145" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>162</v>
       </c>
@@ -19413,7 +19410,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="146" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>22581228</v>
       </c>
@@ -19514,7 +19511,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="147" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>22238593</v>
       </c>
@@ -19615,7 +19612,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>22556366</v>
       </c>
@@ -19716,7 +19713,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="149" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>22446960</v>
       </c>
@@ -19817,7 +19814,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="150" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>22539988</v>
       </c>
@@ -19918,7 +19915,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>23041452</v>
       </c>
@@ -20019,7 +20016,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="152" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>23152477</v>
       </c>
@@ -20120,7 +20117,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>22698912</v>
       </c>
@@ -20221,7 +20218,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="154" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>23144628</v>
       </c>
@@ -20322,7 +20319,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="155" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>22885924</v>
       </c>
@@ -20423,7 +20420,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>22885922</v>
       </c>
@@ -20524,7 +20521,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>22325160</v>
       </c>
@@ -20625,7 +20622,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>22544366</v>
       </c>
@@ -20726,7 +20723,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>22479202</v>
       </c>
@@ -20827,7 +20824,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>22607825</v>
       </c>
@@ -20849,7 +20846,7 @@
       <c r="G160" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="H160" s="10" t="s">
+      <c r="H160" s="3" t="s">
         <v>594</v>
       </c>
       <c r="I160" s="8">
@@ -20928,7 +20925,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>22264825</v>
       </c>
@@ -21029,7 +21026,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="162" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>22693455</v>
       </c>
@@ -21130,7 +21127,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>22876189</v>
       </c>
@@ -21231,7 +21228,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>21606135</v>
       </c>
@@ -21332,7 +21329,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>21597005</v>
       </c>
@@ -21433,7 +21430,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="166" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>162</v>
       </c>
@@ -21534,7 +21531,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>21909115</v>
       </c>
@@ -21635,7 +21632,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="168" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>21423719</v>
       </c>
@@ -21736,7 +21733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="169" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>21873549</v>
       </c>
@@ -21837,7 +21834,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="170" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>22144573</v>
       </c>
@@ -21938,7 +21935,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="171" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>21909110</v>
       </c>
@@ -22039,7 +22036,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="172" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>21757122</v>
       </c>
@@ -22140,7 +22137,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="173" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>21378990</v>
       </c>
@@ -22241,7 +22238,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="174" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>21852963</v>
       </c>
@@ -22342,7 +22339,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="175" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>21308769</v>
       </c>
@@ -22443,7 +22440,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="176" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>21408211</v>
       </c>
@@ -22544,7 +22541,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="177" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>20935630</v>
       </c>
@@ -22645,7 +22642,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="178" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>20686565</v>
       </c>
@@ -22746,7 +22743,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>20858683</v>
       </c>
@@ -22847,7 +22844,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="180" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>20923989</v>
       </c>
@@ -22948,7 +22945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="181" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>20657596</v>
       </c>
@@ -23049,7 +23046,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="182" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>20081857</v>
       </c>
@@ -23150,7 +23147,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="183" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>20418890</v>
       </c>
@@ -23251,7 +23248,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="184" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>20881960</v>
       </c>
@@ -23352,7 +23349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="185" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>20933357</v>
       </c>
@@ -23453,7 +23450,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="186" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>20935629</v>
       </c>
@@ -23554,7 +23551,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="187" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>20838612</v>
       </c>
@@ -23655,7 +23652,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="188" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>20081858</v>
       </c>
@@ -23756,7 +23753,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="189" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>20648472</v>
       </c>
@@ -23857,7 +23854,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="190" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>20581827</v>
       </c>
@@ -23958,7 +23955,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>19820697</v>
       </c>
@@ -24059,7 +24056,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="192" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>19553259</v>
       </c>
@@ -24160,7 +24157,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="193" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>19060906</v>
       </c>
@@ -24261,7 +24258,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="194" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>19198609</v>
       </c>
@@ -24362,7 +24359,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="195" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>19430483</v>
       </c>
@@ -24463,7 +24460,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="196" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>19389826</v>
       </c>
@@ -24564,7 +24561,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="197" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>19198612</v>
       </c>
@@ -24665,7 +24662,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="198" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>19377085</v>
       </c>
@@ -24766,7 +24763,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="199" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>19602701</v>
       </c>
@@ -24867,7 +24864,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="200" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>19060907</v>
       </c>
@@ -24968,7 +24965,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="201" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>18678614</v>
       </c>
@@ -25069,7 +25066,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="202" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>18454148</v>
       </c>
@@ -25170,7 +25167,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="203" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>18391950</v>
       </c>
@@ -25271,7 +25268,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="204" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>18372903</v>
       </c>
@@ -25372,7 +25369,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="205" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>18852200</v>
       </c>
@@ -25473,7 +25470,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="206" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>18193044</v>
       </c>
@@ -25574,7 +25571,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="207" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>17767157</v>
       </c>
@@ -25675,7 +25672,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="208" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>17159977</v>
       </c>
@@ -25776,7 +25773,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="209" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>17463246</v>
       </c>
@@ -25877,7 +25874,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="210" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>16494531</v>
       </c>
@@ -25978,7 +25975,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="211" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>16680197</v>
       </c>
@@ -26079,7 +26076,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="212" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>16151517</v>
       </c>
@@ -26180,7 +26177,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="213" spans="1:33" s="7" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:33" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>16352722</v>
       </c>
@@ -26293,7 +26290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update to sources r2
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1504" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97382EEB-86AE-5048-92C9-BB22C264E02B}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="3200" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="820" yWindow="1040" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4742,7 +4742,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@5cb274e3cf72e9e0e7faca478e361d68f1866a01 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1504" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97382EEB-86AE-5048-92C9-BB22C264E02B}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="3200" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="820" yWindow="1040" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4742,7 +4742,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@3821ca128fa2e8f1f242e07661dbe5728b9ac250 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1504" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97382EEB-86AE-5048-92C9-BB22C264E02B}"/>
+  <xr:revisionPtr revIDLastSave="1507" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BF92D8C-D35E-E54D-9D1A-62B63E34CB25}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="1040" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="626">
   <si>
     <t>10.1186/s13059-023-03136-z</t>
   </si>
@@ -1915,7 +1915,10 @@
     <t>Major Depressive Disorder Impacts Peripheral Artery Disease Risk Through Intermediary Risk Factors</t>
   </si>
   <si>
-    <t>images/covers/PMID_38374256_Cover_artonly.jpg</t>
+    <t>https://github.com/bvoightlab/bvoightlab.github.io/blob/e34920f1f98cf3c1c0907822820d8d51ac93d407/images/covers/PMID_38374256_Cover_artonly.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>https://media.springernature.com/w440/springer-static/cover-hires/journal/41588/49/6</t>
   </si>
 </sst>
 </file>
@@ -4741,8 +4744,8 @@
   <dimension ref="A1:AG215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -16201,7 +16204,7 @@
         <v>64</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>162</v>
+        <v>625</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>496</v>

</xml_diff>

<commit_message>
update to image (Johnson et al)
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1507" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BF92D8C-D35E-E54D-9D1A-62B63E34CB25}"/>
+  <xr:revisionPtr revIDLastSave="1508" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73763DE8-1C42-7C46-9E27-689704E97A6F}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="1040" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="7980" yWindow="2780" windowWidth="38940" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="627">
   <si>
     <t>10.1186/s13059-023-03136-z</t>
   </si>
@@ -1919,6 +1919,9 @@
   </si>
   <si>
     <t>https://media.springernature.com/w440/springer-static/cover-hires/journal/41588/49/6</t>
+  </si>
+  <si>
+    <t>https://github.com/bvoightlab/bvoightlab.github.io/blob/main/images/covers/JohnsonEA_IBD_Cover_artonly.png?raw=true</t>
   </si>
 </sst>
 </file>
@@ -4744,8 +4747,8 @@
   <dimension ref="A1:AG215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -6609,7 +6612,7 @@
         <v>196</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>162</v>
+        <v>626</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>578</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@15ee19ef20e265f461482d25cd8cce6736841bf6 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1507" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BF92D8C-D35E-E54D-9D1A-62B63E34CB25}"/>
+  <xr:revisionPtr revIDLastSave="1508" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73763DE8-1C42-7C46-9E27-689704E97A6F}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="1040" windowWidth="55960" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="7980" yWindow="2780" windowWidth="38940" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6249" uniqueCount="627">
   <si>
     <t>10.1186/s13059-023-03136-z</t>
   </si>
@@ -1919,6 +1919,9 @@
   </si>
   <si>
     <t>https://media.springernature.com/w440/springer-static/cover-hires/journal/41588/49/6</t>
+  </si>
+  <si>
+    <t>https://github.com/bvoightlab/bvoightlab.github.io/blob/main/images/covers/JohnsonEA_IBD_Cover_artonly.png?raw=true</t>
   </si>
 </sst>
 </file>
@@ -4744,8 +4747,8 @@
   <dimension ref="A1:AG215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -6609,7 +6612,7 @@
         <v>196</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>162</v>
+        <v>626</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>578</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ bvoightlab/bvoightlab.github.io@f329541a35f6a63862e30c3de9be7377a2046ad9 🚀
</commit_message>
<xml_diff>
--- a/mydata/Voight_publication_doi_taglist.xlsx
+++ b/mydata/Voight_publication_doi_taglist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4816d84074173a69/My_So_Called_Life/Website/bvoightlab_website_v4.0/mydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1508" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73763DE8-1C42-7C46-9E27-689704E97A6F}"/>
+  <xr:revisionPtr revIDLastSave="1509" documentId="8_{342E141F-12AE-5D4E-A7C8-D0497FDA344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D535BBFE-AB0F-9E42-9882-FAC854D4D78D}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="2780" windowWidth="38940" windowHeight="29620" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
+    <workbookView xWindow="2040" yWindow="2280" windowWidth="34320" windowHeight="28360" activeTab="1" xr2:uid="{A6B2F514-4A42-BB4D-A1B7-F3C87B3AD4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1369,9 +1369,6 @@
     <t>Multi-Trait Genome-Wide Association Study of Atherosclerosis Detects Novel Pleiotropic Loci</t>
   </si>
   <si>
-    <t>Polygenic Risk Scores in Alzheimeru2019s Disease Genetics: MethodologyApplications  Inclusion  and Diversity</t>
-  </si>
-  <si>
     <t>Mendelian randomization analyses clarify the effects of height on cardiovascular diseases</t>
   </si>
   <si>
@@ -1922,6 +1919,9 @@
   </si>
   <si>
     <t>https://github.com/bvoightlab/bvoightlab.github.io/blob/main/images/covers/JohnsonEA_IBD_Cover_artonly.png?raw=true</t>
+  </si>
+  <si>
+    <t>Polygenic Risk Scores in Alzheimers Disease Genetics: MethodologyApplications  Inclusion  and Diversity</t>
   </si>
 </sst>
 </file>
@@ -2025,14 +2025,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2070,7 +2066,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2176,7 +2172,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2318,7 +2314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4747,8 +4743,8 @@
   <dimension ref="A1:AG215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -4794,7 +4790,7 @@
         <v>187</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>190</v>
@@ -4812,28 +4808,28 @@
         <v>415</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>164</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>570</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>571</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>169</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>171</v>
@@ -4845,7 +4841,7 @@
         <v>173</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U1" s="8" t="s">
         <v>175</v>
@@ -4869,19 +4865,19 @@
         <v>181</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AC1" s="8" t="s">
         <v>183</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AE1" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AF1" s="8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AG1" s="8" t="s">
         <v>403</v>
@@ -4892,13 +4888,13 @@
         <v>38362853</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>622</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>623</v>
       </c>
       <c r="E2" s="3">
         <v>2024</v>
@@ -4993,13 +4989,13 @@
         <v>38374256</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>621</v>
       </c>
       <c r="E3" s="3">
         <v>2024</v>
@@ -5813,7 +5809,7 @@
         <v>2022</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>162</v>
@@ -6208,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>430</v>
@@ -6217,7 +6213,7 @@
         <v>2023</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>162</v>
@@ -6312,7 +6308,7 @@
         <v>162</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E16" s="3">
         <v>2023</v>
@@ -6612,19 +6608,19 @@
         <v>196</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E19" s="3">
         <v>2022</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>162</v>
@@ -6722,7 +6718,7 @@
         <v>2022</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>162</v>
@@ -6814,7 +6810,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>433</v>
@@ -6823,10 +6819,10 @@
         <v>2022</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>162</v>
@@ -6924,7 +6920,7 @@
         <v>2022</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>162</v>
@@ -7016,7 +7012,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>434</v>
@@ -7028,7 +7024,7 @@
         <v>162</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>162</v>
@@ -7120,7 +7116,7 @@
         <v>162</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E24" s="3">
         <v>2022</v>
@@ -7129,7 +7125,7 @@
         <v>162</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>162</v>
@@ -7218,7 +7214,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>435</v>
@@ -7230,7 +7226,7 @@
         <v>162</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>162</v>
@@ -7319,7 +7315,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>436</v>
@@ -7331,7 +7327,7 @@
         <v>162</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>162</v>
@@ -7521,7 +7517,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>438</v>
@@ -7928,7 +7924,7 @@
         <v>162</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>442</v>
+        <v>626</v>
       </c>
       <c r="E32" s="3">
         <v>2022</v>
@@ -8130,7 +8126,7 @@
         <v>162</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E34" s="3">
         <v>2021</v>
@@ -8231,7 +8227,7 @@
         <v>162</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E35" s="3">
         <v>2021</v>
@@ -8338,7 +8334,7 @@
         <v>2021</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>162</v>
@@ -8635,7 +8631,7 @@
         <v>162</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E39" s="3">
         <v>2021</v>
@@ -8736,7 +8732,7 @@
         <v>162</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E40" s="3">
         <v>2021</v>
@@ -8837,7 +8833,7 @@
         <v>162</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E41" s="3">
         <v>2021</v>
@@ -8938,7 +8934,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E42" s="3">
         <v>2021</v>
@@ -9140,7 +9136,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E44" s="3">
         <v>2021</v>
@@ -9241,7 +9237,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E45" s="3">
         <v>2021</v>
@@ -9342,7 +9338,7 @@
         <v>162</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E46" s="3">
         <v>2021</v>
@@ -9443,7 +9439,7 @@
         <v>162</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E47" s="3">
         <v>2021</v>
@@ -9544,7 +9540,7 @@
         <v>162</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E48" s="3">
         <v>2020</v>
@@ -9645,7 +9641,7 @@
         <v>162</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E49" s="3">
         <v>2021</v>
@@ -9847,7 +9843,7 @@
         <v>162</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E51" s="3">
         <v>2021</v>
@@ -10049,7 +10045,7 @@
         <v>162</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E53" s="3">
         <v>2021</v>
@@ -10150,7 +10146,7 @@
         <v>162</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E54" s="3">
         <v>2020</v>
@@ -10251,7 +10247,7 @@
         <v>162</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E55" s="3">
         <v>2021</v>
@@ -10352,7 +10348,7 @@
         <v>162</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E56" s="3">
         <v>2021</v>
@@ -10453,7 +10449,7 @@
         <v>162</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E57" s="3">
         <v>2021</v>
@@ -10554,7 +10550,7 @@
         <v>162</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E58" s="3">
         <v>2021</v>
@@ -10857,7 +10853,7 @@
         <v>162</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E61" s="3">
         <v>2020</v>
@@ -10958,7 +10954,7 @@
         <v>162</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E62" s="3">
         <v>2020</v>
@@ -11059,7 +11055,7 @@
         <v>162</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E63" s="3">
         <v>2020</v>
@@ -11160,13 +11156,13 @@
         <v>162</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E64" s="3">
         <v>2020</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>162</v>
@@ -11261,7 +11257,7 @@
         <v>162</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E65" s="3">
         <v>2020</v>
@@ -11362,7 +11358,7 @@
         <v>162</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E66" s="3">
         <v>2020</v>
@@ -11463,13 +11459,13 @@
         <v>162</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E67" s="3">
         <v>2020</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>162</v>
@@ -11564,7 +11560,7 @@
         <v>162</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E68" s="3">
         <v>2020</v>
@@ -11665,7 +11661,7 @@
         <v>162</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E69" s="3">
         <v>2020</v>
@@ -11766,7 +11762,7 @@
         <v>162</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E70" s="3">
         <v>2020</v>
@@ -11867,7 +11863,7 @@
         <v>162</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E71" s="3">
         <v>2019</v>
@@ -11968,7 +11964,7 @@
         <v>162</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E72" s="3">
         <v>2020</v>
@@ -12170,7 +12166,7 @@
         <v>162</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E74" s="3">
         <v>2020</v>
@@ -12271,7 +12267,7 @@
         <v>162</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E75" s="3">
         <v>2020</v>
@@ -12372,7 +12368,7 @@
         <v>162</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E76" s="3">
         <v>2020</v>
@@ -12473,7 +12469,7 @@
         <v>162</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E77" s="3">
         <v>2020</v>
@@ -12675,7 +12671,7 @@
         <v>162</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E79" s="3">
         <v>2020</v>
@@ -12776,7 +12772,7 @@
         <v>162</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E80" s="3">
         <v>2020</v>
@@ -12877,7 +12873,7 @@
         <v>162</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E81" s="3">
         <v>2019</v>
@@ -13079,7 +13075,7 @@
         <v>162</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E83" s="3">
         <v>2019</v>
@@ -13180,7 +13176,7 @@
         <v>162</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E84" s="3">
         <v>2019</v>
@@ -13281,7 +13277,7 @@
         <v>162</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E85" s="3">
         <v>2019</v>
@@ -13382,7 +13378,7 @@
         <v>162</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E86" s="3">
         <v>2019</v>
@@ -13483,7 +13479,7 @@
         <v>162</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E87" s="3">
         <v>2019</v>
@@ -13584,7 +13580,7 @@
         <v>162</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E88" s="3">
         <v>2019</v>
@@ -13685,7 +13681,7 @@
         <v>162</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E89" s="3">
         <v>2019</v>
@@ -13786,7 +13782,7 @@
         <v>162</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E90" s="3">
         <v>2019</v>
@@ -13988,13 +13984,13 @@
         <v>162</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E92" s="3">
         <v>2018</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>162</v>
@@ -14190,7 +14186,7 @@
         <v>162</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E94" s="3">
         <v>2018</v>
@@ -14392,7 +14388,7 @@
         <v>162</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E96" s="3">
         <v>2018</v>
@@ -14493,7 +14489,7 @@
         <v>162</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E97" s="3">
         <v>2018</v>
@@ -14594,7 +14590,7 @@
         <v>162</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E98" s="3">
         <v>2018</v>
@@ -14695,7 +14691,7 @@
         <v>162</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E99" s="3">
         <v>2017</v>
@@ -14796,7 +14792,7 @@
         <v>162</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E100" s="3">
         <v>2018</v>
@@ -15099,7 +15095,7 @@
         <v>162</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E103" s="3">
         <v>2017</v>
@@ -15200,7 +15196,7 @@
         <v>162</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E104" s="3">
         <v>2017</v>
@@ -15307,7 +15303,7 @@
         <v>2017</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>162</v>
@@ -15408,7 +15404,7 @@
         <v>2017</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>162</v>
@@ -15604,7 +15600,7 @@
         <v>162</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E108" s="3">
         <v>2017</v>
@@ -15705,7 +15701,7 @@
         <v>162</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E109" s="3">
         <v>2017</v>
@@ -15806,7 +15802,7 @@
         <v>162</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E110" s="3">
         <v>2017</v>
@@ -15907,7 +15903,7 @@
         <v>162</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E111" s="3">
         <v>2017</v>
@@ -16109,7 +16105,7 @@
         <v>162</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E113" s="3">
         <v>2016</v>
@@ -16207,10 +16203,10 @@
         <v>64</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E114" s="3">
         <v>2017</v>
@@ -16311,7 +16307,7 @@
         <v>162</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E115" s="3">
         <v>2016</v>
@@ -16412,7 +16408,7 @@
         <v>162</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E116" s="3">
         <v>2016</v>
@@ -16513,7 +16509,7 @@
         <v>162</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E117" s="3">
         <v>2016</v>
@@ -16614,7 +16610,7 @@
         <v>162</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E118" s="3">
         <v>2016</v>
@@ -17018,7 +17014,7 @@
         <v>162</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E122" s="3">
         <v>2016</v>
@@ -17220,7 +17216,7 @@
         <v>162</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E124" s="3">
         <v>2016</v>
@@ -17422,7 +17418,7 @@
         <v>162</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E126" s="3">
         <v>2015</v>
@@ -17523,7 +17519,7 @@
         <v>162</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E127" s="3">
         <v>2015</v>
@@ -17624,7 +17620,7 @@
         <v>162</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E128" s="3">
         <v>2015</v>
@@ -18028,7 +18024,7 @@
         <v>162</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E132" s="3">
         <v>2014</v>
@@ -18337,7 +18333,7 @@
         <v>2014</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>162</v>
@@ -18533,7 +18529,7 @@
         <v>162</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E137" s="3">
         <v>2014</v>
@@ -18735,7 +18731,7 @@
         <v>162</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E139" s="3">
         <v>2013</v>
@@ -19038,7 +19034,7 @@
         <v>162</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E142" s="3">
         <v>2013</v>
@@ -19240,7 +19236,7 @@
         <v>162</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E144" s="3">
         <v>2012</v>
@@ -19341,7 +19337,7 @@
         <v>162</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E145" s="3">
         <v>2013</v>
@@ -19644,7 +19640,7 @@
         <v>162</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E148" s="3">
         <v>2012</v>
@@ -20048,7 +20044,7 @@
         <v>162</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E152" s="3">
         <v>2012</v>
@@ -20149,7 +20145,7 @@
         <v>162</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E153" s="3">
         <v>2012</v>
@@ -20250,7 +20246,7 @@
         <v>162</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E154" s="3">
         <v>2012</v>
@@ -20351,7 +20347,7 @@
         <v>162</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E155" s="3">
         <v>2012</v>
@@ -20452,7 +20448,7 @@
         <v>162</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E156" s="3">
         <v>2012</v>
@@ -20553,7 +20549,7 @@
         <v>162</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E157" s="3">
         <v>2012</v>
@@ -20654,7 +20650,7 @@
         <v>162</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E158" s="3">
         <v>2012</v>
@@ -20755,7 +20751,7 @@
         <v>162</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E159" s="3">
         <v>2012</v>
@@ -20957,7 +20953,7 @@
         <v>162</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E161" s="3">
         <v>2012</v>
@@ -21055,10 +21051,10 @@
         <v>97</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E162" s="3">
         <v>2012</v>
@@ -21067,10 +21063,10 @@
         <v>162</v>
       </c>
       <c r="G162" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="H162" s="3" t="s">
         <v>593</v>
-      </c>
-      <c r="H162" s="3" t="s">
-        <v>594</v>
       </c>
       <c r="I162" s="8">
         <v>1</v>
@@ -21159,7 +21155,7 @@
         <v>162</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E163" s="3">
         <v>2012</v>
@@ -21260,7 +21256,7 @@
         <v>162</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E164" s="3">
         <v>2012</v>
@@ -21361,7 +21357,7 @@
         <v>162</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E165" s="3">
         <v>2012</v>
@@ -21462,7 +21458,7 @@
         <v>162</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E166" s="3">
         <v>2011</v>
@@ -21563,7 +21559,7 @@
         <v>162</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E167" s="3">
         <v>2011</v>
@@ -21765,7 +21761,7 @@
         <v>162</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E169" s="3">
         <v>2011</v>
@@ -21866,7 +21862,7 @@
         <v>162</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E170" s="3">
         <v>2011</v>
@@ -21967,7 +21963,7 @@
         <v>162</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E171" s="3">
         <v>2011</v>
@@ -22068,7 +22064,7 @@
         <v>162</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E172" s="3">
         <v>2011</v>
@@ -22169,7 +22165,7 @@
         <v>162</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E173" s="3">
         <v>2011</v>
@@ -22270,7 +22266,7 @@
         <v>162</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E174" s="3">
         <v>2011</v>
@@ -22371,7 +22367,7 @@
         <v>162</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E175" s="3">
         <v>2011</v>
@@ -22478,7 +22474,7 @@
         <v>2011</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>162</v>
@@ -22573,7 +22569,7 @@
         <v>162</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E177" s="3">
         <v>2011</v>
@@ -22775,7 +22771,7 @@
         <v>162</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E179" s="3">
         <v>2010</v>
@@ -22977,7 +22973,7 @@
         <v>162</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E181" s="3">
         <v>2010</v>
@@ -23078,7 +23074,7 @@
         <v>162</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E182" s="3">
         <v>2010</v>
@@ -23179,7 +23175,7 @@
         <v>162</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E183" s="3">
         <v>2010</v>
@@ -23280,7 +23276,7 @@
         <v>162</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E184" s="3">
         <v>2010</v>
@@ -23381,7 +23377,7 @@
         <v>162</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E185" s="3">
         <v>2010</v>
@@ -23482,7 +23478,7 @@
         <v>162</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E186" s="3">
         <v>2010</v>
@@ -23583,7 +23579,7 @@
         <v>162</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E187" s="3">
         <v>2010</v>
@@ -23684,7 +23680,7 @@
         <v>162</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E188" s="3">
         <v>2010</v>
@@ -23886,7 +23882,7 @@
         <v>162</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E190" s="3">
         <v>2010</v>
@@ -23987,7 +23983,7 @@
         <v>162</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E191" s="3">
         <v>2010</v>
@@ -24088,7 +24084,7 @@
         <v>162</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E192" s="3">
         <v>2010</v>
@@ -24189,7 +24185,7 @@
         <v>162</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E193" s="3">
         <v>2009</v>
@@ -24492,7 +24488,7 @@
         <v>162</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E196" s="3">
         <v>2009</v>
@@ -24593,7 +24589,7 @@
         <v>162</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E197" s="3">
         <v>2009</v>
@@ -24694,7 +24690,7 @@
         <v>162</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E198" s="3">
         <v>2009</v>
@@ -24896,7 +24892,7 @@
         <v>162</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E200" s="3">
         <v>2009</v>
@@ -25199,7 +25195,7 @@
         <v>162</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E203" s="3">
         <v>2008</v>
@@ -25300,7 +25296,7 @@
         <v>162</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E204" s="3">
         <v>2008</v>
@@ -25401,7 +25397,7 @@
         <v>162</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E205" s="3">
         <v>2008</v>
@@ -25502,7 +25498,7 @@
         <v>162</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E206" s="3">
         <v>2008</v>
@@ -25603,7 +25599,7 @@
         <v>162</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E207" s="3">
         <v>2008</v>
@@ -25704,7 +25700,7 @@
         <v>162</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E208" s="3">
         <v>2008</v>
@@ -25802,10 +25798,10 @@
         <v>157</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E209" s="3">
         <v>2007</v>
@@ -25814,7 +25810,7 @@
         <v>162</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H209" s="3" t="s">
         <v>162</v>
@@ -25903,7 +25899,7 @@
         <v>156</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>397</v>
@@ -25915,10 +25911,10 @@
         <v>162</v>
       </c>
       <c r="G210" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="H210" s="3" t="s">
         <v>600</v>
-      </c>
-      <c r="H210" s="3" t="s">
-        <v>601</v>
       </c>
       <c r="I210" s="8">
         <v>1</v>
@@ -26004,10 +26000,10 @@
         <v>155</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E211" s="3">
         <v>2007</v>
@@ -26016,10 +26012,10 @@
         <v>162</v>
       </c>
       <c r="G211" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="H211" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="H211" s="3" t="s">
-        <v>596</v>
       </c>
       <c r="I211" s="8">
         <v>1</v>
@@ -26105,7 +26101,7 @@
         <v>159</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>399</v>
@@ -26114,13 +26110,13 @@
         <v>2006</v>
       </c>
       <c r="F212" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H212" s="3" t="s">
         <v>605</v>
-      </c>
-      <c r="G212" s="3" t="s">
-        <v>604</v>
-      </c>
-      <c r="H212" s="3" t="s">
-        <v>606</v>
       </c>
       <c r="I212" s="8">
         <v>1</v>
@@ -26206,10 +26202,10 @@
         <v>158</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E213" s="3">
         <v>2006</v>
@@ -26218,7 +26214,7 @@
         <v>162</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>162</v>
@@ -26307,7 +26303,7 @@
         <v>161</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>401</v>
@@ -26319,7 +26315,7 @@
         <v>162</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H214" s="3" t="s">
         <v>162</v>
@@ -26408,10 +26404,10 @@
         <v>160</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E215" s="3">
         <v>2005</v>
@@ -26420,7 +26416,7 @@
         <v>162</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>162</v>

</xml_diff>